<commit_message>
Add CO2 emissions from gasoline for private cars and taxis
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Emissions.xlsx
+++ b/SuppXLS/Scen_TRA_Emissions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4E5470-E826-4AB8-97E9-50228772727A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A5E672-5EEB-4F96-BB00-844975886200}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -54,7 +54,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Maurizio Gargiulo</author>
-    <author>Gary Goldstein</author>
   </authors>
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -68,32 +67,6 @@
             <family val="2"/>
           </rPr>
           <t>Insert Table</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AJ2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Define the qualifiers based upon technology set + topology + name + descriptions, according to both include and exclude specifications.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AO2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Define the qualifiers based upon commodity set + name + descriptions, according to both include and exclude specifications.</t>
         </r>
       </text>
     </comment>
@@ -160,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -422,16 +395,16 @@
     <t>FLO_EMIS</t>
   </si>
   <si>
-    <t>TRAPM25</t>
-  </si>
-  <si>
-    <t>other_indexes</t>
-  </si>
-  <si>
     <t>t-car*,t-tax*</t>
   </si>
   <si>
-    <t>TRAGSL_NRGI</t>
+    <t>TRAGSL</t>
+  </si>
+  <si>
+    <t>Other_indexes</t>
+  </si>
+  <si>
+    <t>TRACO2</t>
   </si>
 </sst>
 </file>
@@ -648,7 +621,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>22860</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1026,40 +999,40 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="3.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5546875" style="7" customWidth="1"/>
-    <col min="25" max="25" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" style="7" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.109375" style="7"/>
+    <col min="29" max="29" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -1173,12 +1146,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>45</v>
       </c>
@@ -1293,7 +1266,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>48</v>
       </c>
@@ -1410,7 +1383,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>49</v>
       </c>
@@ -1527,7 +1500,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>50</v>
       </c>
@@ -1535,7 +1508,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>52</v>
       </c>
@@ -1543,7 +1516,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>53</v>
       </c>
@@ -1551,7 +1524,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>54</v>
       </c>
@@ -1559,7 +1532,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>55</v>
       </c>
@@ -1567,7 +1540,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>56</v>
       </c>
@@ -1575,7 +1548,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>57</v>
       </c>
@@ -1583,7 +1556,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>58</v>
       </c>
@@ -1591,7 +1564,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>59</v>
       </c>
@@ -1599,7 +1572,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>60</v>
       </c>
@@ -1607,7 +1580,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>61</v>
       </c>
@@ -1615,7 +1588,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>62</v>
       </c>
@@ -1623,7 +1596,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>63</v>
       </c>
@@ -1631,7 +1604,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>64</v>
       </c>
@@ -1639,7 +1612,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>65</v>
       </c>
@@ -1647,7 +1620,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>66</v>
       </c>
@@ -1655,7 +1628,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>67</v>
       </c>
@@ -1663,7 +1636,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>68</v>
       </c>
@@ -1671,7 +1644,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>69</v>
       </c>
@@ -1679,7 +1652,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>70</v>
       </c>
@@ -1687,7 +1660,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>71</v>
       </c>
@@ -1695,7 +1668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>72</v>
       </c>
@@ -1703,7 +1676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>73</v>
       </c>
@@ -1711,7 +1684,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>74</v>
       </c>
@@ -1719,7 +1692,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>75</v>
       </c>
@@ -1727,7 +1700,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>76</v>
       </c>
@@ -1735,7 +1708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>77</v>
       </c>
@@ -1743,7 +1716,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>78</v>
       </c>
@@ -1769,7 +1742,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -1787,54 +1760,38 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="34" width="10.6640625" customWidth="1"/>
-    <col min="35" max="35" width="10.6640625" style="7" customWidth="1"/>
-    <col min="36" max="36" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AJ2" s="2"/>
-      <c r="AK2" s="3"/>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3"/>
-      <c r="AQ2" s="3"/>
-      <c r="AR2" s="3"/>
-    </row>
-    <row r="3" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1847,166 +1804,34 @@
       <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="5" t="str">
-        <f>Regions!C$3</f>
-        <v>IE</v>
-      </c>
-      <c r="J3" s="5" t="str">
-        <f>Regions!E$3</f>
-        <v>IE-CW</v>
-      </c>
-      <c r="K3" s="5" t="str">
-        <f>Regions!F$3</f>
-        <v>IE-D</v>
-      </c>
-      <c r="L3" s="5" t="str">
-        <f>Regions!G$3</f>
-        <v>IE-KE</v>
-      </c>
-      <c r="M3" s="5" t="str">
-        <f>Regions!H$3</f>
-        <v>IE-KK</v>
-      </c>
-      <c r="N3" s="5" t="str">
-        <f>Regions!I$3</f>
-        <v>IE-LS</v>
-      </c>
-      <c r="O3" s="5" t="str">
-        <f>Regions!J$3</f>
-        <v>IE-LD</v>
-      </c>
-      <c r="P3" s="5" t="str">
-        <f>Regions!K$3</f>
-        <v>IE-LH</v>
-      </c>
-      <c r="Q3" s="5" t="str">
-        <f>Regions!L$3</f>
-        <v>IE-MH</v>
-      </c>
-      <c r="R3" s="5" t="str">
-        <f>Regions!M$3</f>
-        <v>IE-OY</v>
-      </c>
-      <c r="S3" s="5" t="str">
-        <f>Regions!N$3</f>
-        <v>IE-WH</v>
-      </c>
-      <c r="T3" s="5" t="str">
-        <f>Regions!O$3</f>
-        <v>IE-WX</v>
-      </c>
-      <c r="U3" s="5" t="str">
-        <f>Regions!P$3</f>
-        <v>IE-WW</v>
-      </c>
-      <c r="V3" s="5" t="str">
-        <f>Regions!Q$3</f>
-        <v>IE-CE</v>
-      </c>
-      <c r="W3" s="5" t="str">
-        <f>Regions!R$3</f>
-        <v>IE-CO</v>
-      </c>
-      <c r="X3" s="5" t="str">
-        <f>Regions!S$3</f>
-        <v>IE-KY</v>
-      </c>
-      <c r="Y3" s="5" t="str">
-        <f>Regions!T$3</f>
-        <v>IE-LK</v>
-      </c>
-      <c r="Z3" s="5" t="str">
-        <f>Regions!U$3</f>
-        <v>IE-TA</v>
-      </c>
-      <c r="AA3" s="5" t="str">
-        <f>Regions!V$3</f>
-        <v>IE-WD</v>
-      </c>
-      <c r="AB3" s="5" t="str">
-        <f>Regions!W$3</f>
-        <v>IE-G</v>
-      </c>
-      <c r="AC3" s="5" t="str">
-        <f>Regions!X$3</f>
-        <v>IE-LM</v>
-      </c>
-      <c r="AD3" s="5" t="str">
-        <f>Regions!Y$3</f>
-        <v>IE-MO</v>
-      </c>
-      <c r="AE3" s="5" t="str">
-        <f>Regions!Z$3</f>
-        <v>IE-RN</v>
-      </c>
-      <c r="AF3" s="5" t="str">
-        <f>Regions!AA$3</f>
-        <v>IE-SO</v>
-      </c>
-      <c r="AG3" s="5" t="str">
-        <f>Regions!AB$3</f>
-        <v>IE-CN</v>
-      </c>
-      <c r="AH3" s="5" t="str">
-        <f>Regions!AC$3</f>
-        <v>IE-DL</v>
-      </c>
-      <c r="AI3" s="5" t="str">
-        <f>Regions!AD$3</f>
-        <v>IE-MN</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AL3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="AQ3" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AR3" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="I3" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>79</v>
       </c>
-      <c r="E4">
-        <v>2018</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP4" t="s">
+      <c r="F4">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
         <v>80</v>
       </c>
-      <c r="AQ4" s="14" t="s">
+      <c r="H4" t="s">
         <v>83</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2024,30 +1849,30 @@
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="34" width="10.6640625" customWidth="1"/>
-    <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="34" width="10.7109375" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2060,7 +1885,7 @@
       <c r="AO2" s="3"/>
       <c r="AP2" s="3"/>
     </row>
-    <row r="3" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Add TRA CO2 emissions
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Emissions.xlsx
+++ b/SuppXLS/Scen_TRA_Emissions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A5E672-5EEB-4F96-BB00-844975886200}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B21B873-E5E2-4DEB-9275-B1CD5AA6096C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t>IE</t>
-  </si>
-  <si>
-    <t>National</t>
   </si>
   <si>
     <t>Single-region</t>
@@ -395,23 +392,41 @@
     <t>FLO_EMIS</t>
   </si>
   <si>
-    <t>t-car*,t-tax*</t>
-  </si>
-  <si>
     <t>TRAGSL</t>
   </si>
   <si>
     <t>Other_indexes</t>
   </si>
   <si>
-    <t>TRACO2</t>
+    <t>kt/PJ</t>
+  </si>
+  <si>
+    <t>*Unit</t>
+  </si>
+  <si>
+    <t>TRADST</t>
+  </si>
+  <si>
+    <t>TRACNG</t>
+  </si>
+  <si>
+    <t>TRALNG</t>
+  </si>
+  <si>
+    <t>TRAKER</t>
+  </si>
+  <si>
+    <t>TRACO2N</t>
+  </si>
+  <si>
+    <t>*National</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,6 +467,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -562,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -587,6 +609,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -996,7 +1021,7 @@
   <dimension ref="A3:AD37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,115 +1059,115 @@
   <sheetData>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="str" cm="1">
-        <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
+        <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
       </c>
       <c r="D3" s="8" t="str" cm="1">
-        <f t="array" ref="D3">INDEX(D5:D7,$A$4)</f>
-        <v>National</v>
+        <f t="array" ref="D3">IF(LEFT(INDEX(D5:D7,$A$4),1)&lt;&gt;"*",INDEX(D5:D7,$A$4),"")</f>
+        <v/>
       </c>
       <c r="E3" s="8" t="str" cm="1">
-        <f t="array" ref="E3">INDEX(E5:E7,$A$4)</f>
+        <f t="array" ref="E3">IF(LEFT(INDEX(E5:E7,$A$4),1)&lt;&gt;"*",INDEX(E5:E7,$A$4),"")</f>
         <v>IE-CW</v>
       </c>
       <c r="F3" s="8" t="str" cm="1">
-        <f t="array" ref="F3">INDEX(F5:F7,$A$4)</f>
+        <f t="array" ref="F3">IF(LEFT(INDEX(F5:F7,$A$4),1)&lt;&gt;"*",INDEX(F5:F7,$A$4),"")</f>
         <v>IE-D</v>
       </c>
       <c r="G3" s="8" t="str" cm="1">
-        <f t="array" ref="G3">INDEX(G5:G7,$A$4)</f>
+        <f t="array" ref="G3">IF(LEFT(INDEX(G5:G7,$A$4),1)&lt;&gt;"*",INDEX(G5:G7,$A$4),"")</f>
         <v>IE-KE</v>
       </c>
       <c r="H3" s="8" t="str" cm="1">
-        <f t="array" ref="H3">INDEX(H5:H7,$A$4)</f>
+        <f t="array" ref="H3">IF(LEFT(INDEX(H5:H7,$A$4),1)&lt;&gt;"*",INDEX(H5:H7,$A$4),"")</f>
         <v>IE-KK</v>
       </c>
       <c r="I3" s="8" t="str" cm="1">
-        <f t="array" ref="I3">INDEX(I5:I7,$A$4)</f>
+        <f t="array" ref="I3">IF(LEFT(INDEX(I5:I7,$A$4),1)&lt;&gt;"*",INDEX(I5:I7,$A$4),"")</f>
         <v>IE-LS</v>
       </c>
       <c r="J3" s="8" t="str" cm="1">
-        <f t="array" ref="J3">INDEX(J5:J7,$A$4)</f>
+        <f t="array" ref="J3">IF(LEFT(INDEX(J5:J7,$A$4),1)&lt;&gt;"*",INDEX(J5:J7,$A$4),"")</f>
         <v>IE-LD</v>
       </c>
       <c r="K3" s="8" t="str" cm="1">
-        <f t="array" ref="K3">INDEX(K5:K7,$A$4)</f>
+        <f t="array" ref="K3">IF(LEFT(INDEX(K5:K7,$A$4),1)&lt;&gt;"*",INDEX(K5:K7,$A$4),"")</f>
         <v>IE-LH</v>
       </c>
       <c r="L3" s="8" t="str" cm="1">
-        <f t="array" ref="L3">INDEX(L5:L7,$A$4)</f>
+        <f t="array" ref="L3">IF(LEFT(INDEX(L5:L7,$A$4),1)&lt;&gt;"*",INDEX(L5:L7,$A$4),"")</f>
         <v>IE-MH</v>
       </c>
       <c r="M3" s="8" t="str" cm="1">
-        <f t="array" ref="M3">INDEX(M5:M7,$A$4)</f>
+        <f t="array" ref="M3">IF(LEFT(INDEX(M5:M7,$A$4),1)&lt;&gt;"*",INDEX(M5:M7,$A$4),"")</f>
         <v>IE-OY</v>
       </c>
       <c r="N3" s="8" t="str" cm="1">
-        <f t="array" ref="N3">INDEX(N5:N7,$A$4)</f>
+        <f t="array" ref="N3">IF(LEFT(INDEX(N5:N7,$A$4),1)&lt;&gt;"*",INDEX(N5:N7,$A$4),"")</f>
         <v>IE-WH</v>
       </c>
       <c r="O3" s="8" t="str" cm="1">
-        <f t="array" ref="O3">INDEX(O5:O7,$A$4)</f>
+        <f t="array" ref="O3">IF(LEFT(INDEX(O5:O7,$A$4),1)&lt;&gt;"*",INDEX(O5:O7,$A$4),"")</f>
         <v>IE-WX</v>
       </c>
       <c r="P3" s="8" t="str" cm="1">
-        <f t="array" ref="P3">INDEX(P5:P7,$A$4)</f>
+        <f t="array" ref="P3">IF(LEFT(INDEX(P5:P7,$A$4),1)&lt;&gt;"*",INDEX(P5:P7,$A$4),"")</f>
         <v>IE-WW</v>
       </c>
       <c r="Q3" s="8" t="str" cm="1">
-        <f t="array" ref="Q3">INDEX(Q5:Q7,$A$4)</f>
+        <f t="array" ref="Q3">IF(LEFT(INDEX(Q5:Q7,$A$4),1)&lt;&gt;"*",INDEX(Q5:Q7,$A$4),"")</f>
         <v>IE-CE</v>
       </c>
       <c r="R3" s="8" t="str" cm="1">
-        <f t="array" ref="R3">INDEX(R5:R7,$A$4)</f>
+        <f t="array" ref="R3">IF(LEFT(INDEX(R5:R7,$A$4),1)&lt;&gt;"*",INDEX(R5:R7,$A$4),"")</f>
         <v>IE-CO</v>
       </c>
       <c r="S3" s="8" t="str" cm="1">
-        <f t="array" ref="S3">INDEX(S5:S7,$A$4)</f>
+        <f t="array" ref="S3">IF(LEFT(INDEX(S5:S7,$A$4),1)&lt;&gt;"*",INDEX(S5:S7,$A$4),"")</f>
         <v>IE-KY</v>
       </c>
       <c r="T3" s="8" t="str" cm="1">
-        <f t="array" ref="T3">INDEX(T5:T7,$A$4)</f>
+        <f t="array" ref="T3">IF(LEFT(INDEX(T5:T7,$A$4),1)&lt;&gt;"*",INDEX(T5:T7,$A$4),"")</f>
         <v>IE-LK</v>
       </c>
       <c r="U3" s="8" t="str" cm="1">
-        <f t="array" ref="U3">INDEX(U5:U7,$A$4)</f>
+        <f t="array" ref="U3">IF(LEFT(INDEX(U5:U7,$A$4),1)&lt;&gt;"*",INDEX(U5:U7,$A$4),"")</f>
         <v>IE-TA</v>
       </c>
       <c r="V3" s="8" t="str" cm="1">
-        <f t="array" ref="V3">INDEX(V5:V7,$A$4)</f>
+        <f t="array" ref="V3">IF(LEFT(INDEX(V5:V7,$A$4),1)&lt;&gt;"*",INDEX(V5:V7,$A$4),"")</f>
         <v>IE-WD</v>
       </c>
       <c r="W3" s="8" t="str" cm="1">
-        <f t="array" ref="W3">INDEX(W5:W7,$A$4)</f>
+        <f t="array" ref="W3">IF(LEFT(INDEX(W5:W7,$A$4),1)&lt;&gt;"*",INDEX(W5:W7,$A$4),"")</f>
         <v>IE-G</v>
       </c>
       <c r="X3" s="8" t="str" cm="1">
-        <f t="array" ref="X3">INDEX(X5:X7,$A$4)</f>
+        <f t="array" ref="X3">IF(LEFT(INDEX(X5:X7,$A$4),1)&lt;&gt;"*",INDEX(X5:X7,$A$4),"")</f>
         <v>IE-LM</v>
       </c>
       <c r="Y3" s="8" t="str" cm="1">
-        <f t="array" ref="Y3">INDEX(Y5:Y7,$A$4)</f>
+        <f t="array" ref="Y3">IF(LEFT(INDEX(Y5:Y7,$A$4),1)&lt;&gt;"*",INDEX(Y5:Y7,$A$4),"")</f>
         <v>IE-MO</v>
       </c>
       <c r="Z3" s="8" t="str" cm="1">
-        <f t="array" ref="Z3">INDEX(Z5:Z7,$A$4)</f>
+        <f t="array" ref="Z3">IF(LEFT(INDEX(Z5:Z7,$A$4),1)&lt;&gt;"*",INDEX(Z5:Z7,$A$4),"")</f>
         <v>IE-RN</v>
       </c>
       <c r="AA3" s="8" t="str" cm="1">
-        <f t="array" ref="AA3">INDEX(AA5:AA7,$A$4)</f>
+        <f t="array" ref="AA3">IF(LEFT(INDEX(AA5:AA7,$A$4),1)&lt;&gt;"*",INDEX(AA5:AA7,$A$4),"")</f>
         <v>IE-SO</v>
       </c>
       <c r="AB3" s="8" t="str" cm="1">
-        <f t="array" ref="AB3">INDEX(AB5:AB7,$A$4)</f>
+        <f t="array" ref="AB3">IF(LEFT(INDEX(AB5:AB7,$A$4),1)&lt;&gt;"*",INDEX(AB5:AB7,$A$4),"")</f>
         <v>IE-CN</v>
       </c>
       <c r="AC3" s="8" t="str" cm="1">
-        <f t="array" ref="AC3">INDEX(AC5:AC7,$A$4)</f>
+        <f t="array" ref="AC3">IF(LEFT(INDEX(AC5:AC7,$A$4),1)&lt;&gt;"*",INDEX(AC5:AC7,$A$4),"")</f>
         <v>IE-DL</v>
       </c>
       <c r="AD3" s="8" t="str" cm="1">
-        <f t="array" ref="AD3">INDEX(AD5:AD7,$A$4)</f>
+        <f t="array" ref="AD3">IF(LEFT(INDEX(AD5:AD7,$A$4),1)&lt;&gt;"*",INDEX(AD5:AD7,$A$4),"")</f>
         <v>IE-MN</v>
       </c>
     </row>
@@ -1150,6 +1175,34 @@
       <c r="A4" s="7">
         <v>1</v>
       </c>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -1159,7 +1212,7 @@
         <v>46</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="E5" s="8" t="str">
         <f>Regions!A11</f>
@@ -1268,18 +1321,18 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="8" t="str">
         <f>C5</f>
         <v>IE</v>
       </c>
       <c r="D6" s="8" t="str">
-        <f>"*"&amp;D5</f>
+        <f>IF(LEFT(D5,1)&lt;&gt;"*","*"&amp;D5,D5)</f>
         <v>*National</v>
       </c>
       <c r="E6" s="8" t="str">
-        <f t="shared" ref="E6:AD6" si="0">"*"&amp;E5</f>
+        <f t="shared" ref="E6:AD6" si="0">IF(LEFT(E5,1)&lt;&gt;"*","*"&amp;E5,E5)</f>
         <v>*IE-CW</v>
       </c>
       <c r="F6" s="8" t="str">
@@ -1385,7 +1438,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="8" t="str">
         <f>"*"&amp;C5</f>
@@ -1393,7 +1446,7 @@
       </c>
       <c r="D7" s="8" t="str">
         <f>D5</f>
-        <v>National</v>
+        <v>*National</v>
       </c>
       <c r="E7" s="8" t="str">
         <f t="shared" ref="E7:AD7" si="1">E5</f>
@@ -1502,15 +1555,15 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>44</v>
@@ -1518,7 +1571,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>43</v>
@@ -1526,7 +1579,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>42</v>
@@ -1534,7 +1587,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>41</v>
@@ -1542,7 +1595,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>40</v>
@@ -1550,7 +1603,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>39</v>
@@ -1558,7 +1611,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>38</v>
@@ -1566,7 +1619,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>37</v>
@@ -1574,7 +1627,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>36</v>
@@ -1582,7 +1635,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>35</v>
@@ -1590,7 +1643,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>34</v>
@@ -1598,7 +1651,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>33</v>
@@ -1606,7 +1659,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>32</v>
@@ -1614,7 +1667,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>31</v>
@@ -1622,7 +1675,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>30</v>
@@ -1630,7 +1683,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>29</v>
@@ -1638,7 +1691,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>28</v>
@@ -1646,7 +1699,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>27</v>
@@ -1654,7 +1707,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>26</v>
@@ -1662,7 +1715,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>25</v>
@@ -1670,7 +1723,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>24</v>
@@ -1678,7 +1731,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>23</v>
@@ -1686,7 +1739,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>22</v>
@@ -1694,7 +1747,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>21</v>
@@ -1702,7 +1755,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>20</v>
@@ -1710,7 +1763,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>19</v>
@@ -1718,7 +1771,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1760,10 +1813,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:AK8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,18 +1825,37 @@
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1791,7 +1863,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1804,33 +1876,773 @@
       <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="F3" s="5" t="str">
+        <f>IF(Regions!C3&lt;&gt;"",Regions!C3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G3" s="5" t="str">
+        <f>IF(Regions!D3&lt;&gt;"",Regions!D3,"*")</f>
+        <v>*</v>
+      </c>
+      <c r="H3" s="5" t="str">
+        <f>IF(Regions!E3&lt;&gt;"",Regions!E3,"*")</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="I3" s="5" t="str">
+        <f>IF(Regions!F3&lt;&gt;"",Regions!F3,"*")</f>
+        <v>IE-D</v>
+      </c>
+      <c r="J3" s="5" t="str">
+        <f>IF(Regions!G3&lt;&gt;"",Regions!G3,"*")</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="K3" s="5" t="str">
+        <f>IF(Regions!H3&lt;&gt;"",Regions!H3,"*")</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="L3" s="5" t="str">
+        <f>IF(Regions!I3&lt;&gt;"",Regions!I3,"*")</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="M3" s="5" t="str">
+        <f>IF(Regions!J3&lt;&gt;"",Regions!J3,"*")</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="N3" s="5" t="str">
+        <f>IF(Regions!K3&lt;&gt;"",Regions!K3,"*")</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="O3" s="5" t="str">
+        <f>IF(Regions!L3&lt;&gt;"",Regions!L3,"*")</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="P3" s="5" t="str">
+        <f>IF(Regions!M3&lt;&gt;"",Regions!M3,"*")</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="Q3" s="5" t="str">
+        <f>IF(Regions!N3&lt;&gt;"",Regions!N3,"*")</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="R3" s="5" t="str">
+        <f>IF(Regions!O3&lt;&gt;"",Regions!O3,"*")</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="S3" s="5" t="str">
+        <f>IF(Regions!P3&lt;&gt;"",Regions!P3,"*")</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="T3" s="5" t="str">
+        <f>IF(Regions!Q3&lt;&gt;"",Regions!Q3,"*")</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="U3" s="5" t="str">
+        <f>IF(Regions!R3&lt;&gt;"",Regions!R3,"*")</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="V3" s="5" t="str">
+        <f>IF(Regions!S3&lt;&gt;"",Regions!S3,"*")</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="W3" s="5" t="str">
+        <f>IF(Regions!T3&lt;&gt;"",Regions!T3,"*")</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="X3" s="5" t="str">
+        <f>IF(Regions!U3&lt;&gt;"",Regions!U3,"*")</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="Y3" s="5" t="str">
+        <f>IF(Regions!V3&lt;&gt;"",Regions!V3,"*")</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="Z3" s="5" t="str">
+        <f>IF(Regions!W3&lt;&gt;"",Regions!W3,"*")</f>
+        <v>IE-G</v>
+      </c>
+      <c r="AA3" s="5" t="str">
+        <f>IF(Regions!X3&lt;&gt;"",Regions!X3,"*")</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="AB3" s="5" t="str">
+        <f>IF(Regions!Y3&lt;&gt;"",Regions!Y3,"*")</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="AC3" s="5" t="str">
+        <f>IF(Regions!Z3&lt;&gt;"",Regions!Z3,"*")</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AD3" s="5" t="str">
+        <f>IF(Regions!AA3&lt;&gt;"",Regions!AA3,"*")</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AE3" s="5" t="str">
+        <f>IF(Regions!AB3&lt;&gt;"",Regions!AB3,"*")</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AF3" s="5" t="str">
+        <f>IF(Regions!AC3&lt;&gt;"",Regions!AC3,"*")</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AG3" s="5" t="str">
+        <f>IF(Regions!AD3&lt;&gt;"",Regions!AD3,"*")</f>
+        <v>IE-MN</v>
+      </c>
+      <c r="AH3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="AJ3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK3" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4">
+        <v>69.3</v>
+      </c>
+      <c r="G4" s="14">
+        <f>$F4</f>
+        <v>69.3</v>
+      </c>
+      <c r="H4" s="14">
+        <f t="shared" ref="H4:AG8" si="0">$F4</f>
+        <v>69.3</v>
+      </c>
+      <c r="I4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="K4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="L4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="M4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="N4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="O4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="P4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="Q4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="R4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="S4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="T4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="U4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="V4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="W4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="X4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="Y4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="Z4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="AA4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="AB4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="AC4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="AD4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="AE4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="AF4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="AG4" s="14">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="AH4" t="str">
+        <f>AJ4</f>
+        <v>TRAGSL</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ4" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F4">
-        <v>70</v>
-      </c>
-      <c r="G4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="AK4" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="G5" s="14">
+        <f t="shared" ref="G5:V8" si="1">$F5</f>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="H5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="I5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="K5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="L5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="M5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="N5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="O5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="P5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="Q5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="R5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="S5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="T5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="U5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="V5" s="14">
+        <f t="shared" si="1"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="W5" s="14">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="X5" s="14">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="Y5" s="14">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="Z5" s="14">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="AA5" s="14">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="AB5" s="14">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="AC5" s="14">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="AD5" s="14">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="AE5" s="14">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="AF5" s="14">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="AG5" s="14">
+        <f t="shared" si="0"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="AH5" s="14" t="str">
+        <f t="shared" ref="AH5:AH8" si="2">AJ5</f>
+        <v>TRADST</v>
+      </c>
+      <c r="AI5" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ5" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="AK5" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6">
+        <v>56.1</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" si="1"/>
+        <v>56.1</v>
+      </c>
+      <c r="H6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="I6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="L6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="M6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="N6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="O6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="P6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="Q6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="R6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="S6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="T6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="U6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="V6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="W6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="X6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="Y6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="Z6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AA6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AB6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AC6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AD6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AE6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AF6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AG6" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AH6" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>TRACNG</v>
+      </c>
+      <c r="AI6" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ6" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK6" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D7" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="14">
+        <v>56.1</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="1"/>
+        <v>56.1</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="N7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="O7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="P7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="Q7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="R7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="S7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="T7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="U7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="V7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="W7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="X7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="Y7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="Z7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AA7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AB7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AC7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AD7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AE7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AF7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AG7" s="14">
+        <f t="shared" si="0"/>
+        <v>56.1</v>
+      </c>
+      <c r="AH7" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>TRALNG</v>
+      </c>
+      <c r="AI7" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ7" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK7" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D8" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="G8" s="14">
+        <f t="shared" si="1"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="H8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="I8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="K8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="N8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="O8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="P8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="Q8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="R8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="S8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="T8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="U8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="V8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="W8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="X8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="Y8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="Z8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="AA8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="AB8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="AC8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="AD8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="AE8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="AF8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="AG8" s="14">
+        <f t="shared" si="0"/>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="AH8" s="14" t="str">
+        <f t="shared" si="2"/>
+        <v>TRAKER</v>
+      </c>
+      <c r="AI8" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ8" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK8" s="15" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>